<commit_message>
Enhance ELECTRE Notebook with Detailed Normalization and Matrix Calculations
- Added vector normalization formula and special handling for minimization criteria in the decision matrix normalization section.
- Updated the code to display normalized and weighted normalized matrices in a structured format.
- Improved output formatting for concordance and discordance matrices, including interpretation notes.
- Adjusted thresholds for concordance and discordance to 0.5 for better decision-making clarity.
- Refined the summary of ELECTRE I results, including clearer presentation of outranking relations and kernel alternatives.
- Removed redundant print statements for cleaner output.
</commit_message>
<xml_diff>
--- a/data/01_examples_with_answer.xlsx
+++ b/data/01_examples_with_answer.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Desktop\code\mcdm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CE21DB-6DCD-418A-A2D8-C0AB1595BD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35130070-FD82-4B7D-9F85-3259716CEB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="16629" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAW" sheetId="1" r:id="rId1"/>
     <sheet name="AHP" sheetId="2" r:id="rId2"/>
     <sheet name="ANP" sheetId="3" r:id="rId3"/>
     <sheet name="TOPSIS" sheetId="4" r:id="rId4"/>
+    <sheet name="ELECTRE" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">AHP!$I$35:$I$39</definedName>
@@ -67,8 +68,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="186">
   <si>
     <t>Decision Matrix</t>
   </si>
@@ -467,6 +490,165 @@
   </si>
   <si>
     <t>Step 7: Calculate Closeness Coefficient and Rank Alternatives</t>
+  </si>
+  <si>
+    <t>Construction Cost (M PHP)</t>
+  </si>
+  <si>
+    <t>Population Density</t>
+  </si>
+  <si>
+    <t>Transportation Access</t>
+  </si>
+  <si>
+    <t>Medical Infrastructure</t>
+  </si>
+  <si>
+    <t>Regulatory Compliance</t>
+  </si>
+  <si>
+    <t>Metro Manila</t>
+  </si>
+  <si>
+    <t>Cebu</t>
+  </si>
+  <si>
+    <t>Davao</t>
+  </si>
+  <si>
+    <t>Iloilo</t>
+  </si>
+  <si>
+    <t>Step 2: Determine Criteria Weights</t>
+  </si>
+  <si>
+    <t>Step 3: Normalize Decision Matrix (using vector normalization)</t>
+  </si>
+  <si>
+    <t>Step 4: Get Weighted Normalized Matrix</t>
+  </si>
+  <si>
+    <t>Step 5: Calculate Concordance Indices</t>
+  </si>
+  <si>
+    <t>Compare MM vs Cebu (Alt 0 vs Alt 1)</t>
+  </si>
+  <si>
+    <t>Alt 0 &gt;= Alt 1?</t>
+  </si>
+  <si>
+    <t>Concorance Index (0,1)</t>
+  </si>
+  <si>
+    <t>Compare MM vs Cebu (Alt 0 vs Alt 2)</t>
+  </si>
+  <si>
+    <t>Alt 0 &gt;= Alt 2?</t>
+  </si>
+  <si>
+    <t>Concorance Index (0,2)</t>
+  </si>
+  <si>
+    <t>Concorance Index (3,2)</t>
+  </si>
+  <si>
+    <t>Step 6: Create Concordance Matrix</t>
+  </si>
+  <si>
+    <t>Step 7: Create Discordance Matrix</t>
+  </si>
+  <si>
+    <t>7.1 Find overall maximum difference between alternatives</t>
+  </si>
+  <si>
+    <t>Metro Manila vs Cebu (Alt 0 vs 1)</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>Max Diff</t>
+  </si>
+  <si>
+    <t>Compare Iloilo vs Davao (Alt 3 vs Alt 2)</t>
+  </si>
+  <si>
+    <t>Iloilo vs Davao (Alt 3 vs Alt 2)</t>
+  </si>
+  <si>
+    <t>Overall Max Diff</t>
+  </si>
+  <si>
+    <t>(Alt 0 vs 3)</t>
+  </si>
+  <si>
+    <t>7.2 Find Discordance Indices</t>
+  </si>
+  <si>
+    <t>Alt 0 &lt;= Alt 1?</t>
+  </si>
+  <si>
+    <t>Differences</t>
+  </si>
+  <si>
+    <t>Discordant Difference</t>
+  </si>
+  <si>
+    <t>Discordant Index (0,1)</t>
+  </si>
+  <si>
+    <t>7.3 Create Discordance Matrix</t>
+  </si>
+  <si>
+    <t>Step 8: Determine Outranking Relations</t>
+  </si>
+  <si>
+    <t>Concordance threshold</t>
+  </si>
+  <si>
+    <t>Discordance threshold</t>
+  </si>
+  <si>
+    <t>Comparing MM vs Cebu (Alt 0 vs 1)</t>
+  </si>
+  <si>
+    <t>Concordance</t>
+  </si>
+  <si>
+    <t>Discordance</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Compare</t>
+  </si>
+  <si>
+    <t>MM OUTRANKS Cebu?</t>
+  </si>
+  <si>
+    <t>Comparing MM vs Davao (Alt 0 vs 2)</t>
+  </si>
+  <si>
+    <t>Create Outranking Matrix (1= outranks, 0 = does not outrank)</t>
+  </si>
+  <si>
+    <t>Step 9: Rank Alternatives</t>
+  </si>
+  <si>
+    <t>Outranks Count</t>
+  </si>
+  <si>
+    <t>Outranked by Count</t>
   </si>
 </sst>
 </file>
@@ -500,7 +682,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +731,12 @@
         <bgColor rgb="FFFFDBB6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -586,7 +774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,12 +811,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -637,6 +825,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -978,20 +1170,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="K2" s="25" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="K2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
     </row>
     <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -1032,7 +1224,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1053,7 +1245,7 @@
       <c r="G4" s="2">
         <v>7</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="5" t="s">
@@ -1081,7 +1273,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1100,7 +1292,7 @@
       <c r="G5" s="2">
         <v>9</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="24"/>
       <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1126,7 +1318,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1145,7 +1337,7 @@
       <c r="G6" s="2">
         <v>8</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1171,7 +1363,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1190,7 +1382,7 @@
       <c r="G7" s="2">
         <v>10</v>
       </c>
-      <c r="I7" s="23"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1216,7 +1408,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1235,7 +1427,7 @@
       <c r="G8" s="2">
         <v>6</v>
       </c>
-      <c r="I8" s="23"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1261,11 +1453,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1277,31 +1469,31 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="1">
         <v>0.25</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:15" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="1">
         <v>0.3</v>
       </c>
@@ -1328,18 +1520,18 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="1">
         <v>0.2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J13" s="5" t="s">
@@ -1367,18 +1559,18 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="1">
         <v>0.15</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="23"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1404,18 +1596,18 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="1">
         <v>0.1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="23"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="5" t="s">
         <v>12</v>
       </c>
@@ -1442,7 +1634,7 @@
     </row>
     <row r="16" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D16" s="1"/>
-      <c r="I16" s="23"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1468,7 +1660,7 @@
       </c>
     </row>
     <row r="17" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I17" s="23"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1529,7 +1721,7 @@
       </c>
     </row>
     <row r="21" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I21" s="23" t="s">
+      <c r="I21" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J21" s="5" t="s">
@@ -1545,7 +1737,7 @@
       </c>
     </row>
     <row r="22" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I22" s="23"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1559,7 +1751,7 @@
       </c>
     </row>
     <row r="23" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I23" s="23"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="5" t="s">
         <v>12</v>
       </c>
@@ -1573,7 +1765,7 @@
       </c>
     </row>
     <row r="24" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I24" s="23"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="5" t="s">
         <v>13</v>
       </c>
@@ -1587,7 +1779,7 @@
       </c>
     </row>
     <row r="25" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I25" s="23"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="5" t="s">
         <v>14</v>
       </c>
@@ -1618,7 +1810,7 @@
       </c>
     </row>
     <row r="28" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="24" t="s">
         <v>9</v>
       </c>
       <c r="J28" s="5" t="str">
@@ -1633,7 +1825,7 @@
       </c>
     </row>
     <row r="29" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I29" s="23"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="5" t="str">
         <v>Laptop B</v>
       </c>
@@ -1645,7 +1837,7 @@
       </c>
     </row>
     <row r="30" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I30" s="23"/>
+      <c r="I30" s="24"/>
       <c r="J30" s="5" t="str">
         <v>Laptop D</v>
       </c>
@@ -1657,7 +1849,7 @@
       </c>
     </row>
     <row r="31" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I31" s="23"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="5" t="str">
         <v>Laptop E</v>
       </c>
@@ -1669,7 +1861,7 @@
       </c>
     </row>
     <row r="32" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I32" s="23"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="5" t="str">
         <v>Laptop A</v>
       </c>
@@ -1682,11 +1874,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="I4:I8"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="I21:I25"/>
     <mergeCell ref="I28:I32"/>
     <mergeCell ref="A11:C11"/>
@@ -1696,6 +1883,11 @@
     <mergeCell ref="I13:I17"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="I4:I8"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5485,16 +5677,6 @@
     <row r="216" ht="14.6" x14ac:dyDescent="0.4"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="X1:AA1"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="P16:S16"/>
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="X44:AA44"/>
     <mergeCell ref="F17:I17"/>
@@ -5502,6 +5684,16 @@
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="F22:F23"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="P16:S16"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="X1:AA1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -5517,8 +5709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F39CA89-FCAC-4A20-B593-18B9A6B2E6BE}">
   <dimension ref="A1:G163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8060,6 +8252,1998 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC014023-8504-4C6E-827A-566A60E05094}">
+  <dimension ref="A1:F147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D142" sqref="D142"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.3828125" customWidth="1"/>
+    <col min="2" max="2" width="22.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.61328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.53515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2500</v>
+      </c>
+      <c r="C3" s="5">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D3" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F3" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1800</v>
+      </c>
+      <c r="C4" s="5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D4" s="5">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E4" s="5">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1600</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7.8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1400</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10">
+        <v>0.3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11">
+        <v>0.25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13">
+        <v>0.15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="5">
+        <f>1/B3^2</f>
+        <v>1.6E-7</v>
+      </c>
+      <c r="C18" s="5">
+        <f>C3^2</f>
+        <v>96.04000000000002</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="C18:F18" si="0">D3^2</f>
+        <v>90.25</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="0"/>
+        <v>84.639999999999986</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="0"/>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" ref="B19:B21" si="1">1/B4^2</f>
+        <v>3.0864197530864198E-7</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" ref="B19:F19" si="2">C4^2</f>
+        <v>67.239999999999995</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="2"/>
+        <v>77.440000000000012</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="2"/>
+        <v>72.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" si="1"/>
+        <v>3.9062500000000002E-7</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" ref="B20:F20" si="3">C5^2</f>
+        <v>56.25</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="3"/>
+        <v>60.839999999999996</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="3"/>
+        <v>51.84</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="3"/>
+        <v>77.440000000000012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" si="1"/>
+        <v>5.1020408163265302E-7</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" ref="B21:F21" si="4">C6^2</f>
+        <v>46.239999999999995</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="4"/>
+        <v>51.84</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="4"/>
+        <v>42.25</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="4"/>
+        <v>84.639999999999986</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B24" s="5">
+        <f>SUM(B18:B21)</f>
+        <v>1.369471056941295E-6</v>
+      </c>
+      <c r="C24" s="28">
+        <f t="shared" ref="B24:F24" si="5">SUM(C18:C21)</f>
+        <v>265.77000000000004</v>
+      </c>
+      <c r="D24" s="28">
+        <f t="shared" si="5"/>
+        <v>280.37</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" si="5"/>
+        <v>242.73</v>
+      </c>
+      <c r="F24" s="28">
+        <f t="shared" si="5"/>
+        <v>290.58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B27" s="28">
+        <f>SQRT(B24)</f>
+        <v>1.1702440159818358E-3</v>
+      </c>
+      <c r="C27" s="28">
+        <f t="shared" ref="C27:F27" si="6">SQRT(C24)</f>
+        <v>16.302453803032229</v>
+      </c>
+      <c r="D27" s="28">
+        <f t="shared" si="6"/>
+        <v>16.744252745345193</v>
+      </c>
+      <c r="E27" s="28">
+        <f t="shared" si="6"/>
+        <v>15.579794607118542</v>
+      </c>
+      <c r="F27" s="28">
+        <f t="shared" si="6"/>
+        <v>17.046407246103207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="28">
+        <f>(1/B3)/$B$27</f>
+        <v>0.34180905395563987</v>
+      </c>
+      <c r="C30" s="28">
+        <f>C3/$C$27</f>
+        <v>0.60113649873844255</v>
+      </c>
+      <c r="D30" s="28">
+        <f>D3/$D$27</f>
+        <v>0.56735885109241113</v>
+      </c>
+      <c r="E30" s="28">
+        <f>E3/$E$27</f>
+        <v>0.59050842658711566</v>
+      </c>
+      <c r="F30" s="28">
+        <f>F3/$F$27</f>
+        <v>0.43997540899502402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="28">
+        <f t="shared" ref="B31:B33" si="7">(1/B4)/$B$27</f>
+        <v>0.4747347971606109</v>
+      </c>
+      <c r="C31" s="28">
+        <f t="shared" ref="C31:C33" si="8">C4/$C$27</f>
+        <v>0.50299176425053349</v>
+      </c>
+      <c r="D31" s="28">
+        <f t="shared" ref="D31:D33" si="9">D4/$D$27</f>
+        <v>0.52555346206454934</v>
+      </c>
+      <c r="E31" s="28">
+        <f t="shared" ref="E31:E33" si="10">E4/$E$27</f>
+        <v>0.51348558833662228</v>
+      </c>
+      <c r="F31" s="28">
+        <f t="shared" ref="F31:F33" si="11">F4/$F$27</f>
+        <v>0.49863879686102724</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="28">
+        <f t="shared" si="7"/>
+        <v>0.53407664680568734</v>
+      </c>
+      <c r="C32" s="28">
+        <f t="shared" si="8"/>
+        <v>0.46005344291207328</v>
+      </c>
+      <c r="D32" s="28">
+        <f t="shared" si="9"/>
+        <v>0.46583147773903233</v>
+      </c>
+      <c r="E32" s="28">
+        <f t="shared" si="10"/>
+        <v>0.46213702950296009</v>
+      </c>
+      <c r="F32" s="28">
+        <f t="shared" si="11"/>
+        <v>0.51623781322082829</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A33" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="28">
+        <f t="shared" si="7"/>
+        <v>0.61037331063507116</v>
+      </c>
+      <c r="C33" s="28">
+        <f t="shared" si="8"/>
+        <v>0.41711512157361313</v>
+      </c>
+      <c r="D33" s="28">
+        <f t="shared" si="9"/>
+        <v>0.42999828714372212</v>
+      </c>
+      <c r="E33" s="28">
+        <f t="shared" si="10"/>
+        <v>0.41720704052350566</v>
+      </c>
+      <c r="F33" s="28">
+        <f t="shared" si="11"/>
+        <v>0.53970316836722942</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A36" s="5"/>
+      <c r="B36" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="28">
+        <f>B30*$C$10</f>
+        <v>0.10254271618669196</v>
+      </c>
+      <c r="C37" s="28">
+        <f>C30*$C$11</f>
+        <v>0.15028412468461064</v>
+      </c>
+      <c r="D37" s="28">
+        <f>D30*$C$12</f>
+        <v>0.11347177021848223</v>
+      </c>
+      <c r="E37" s="28">
+        <f>E30*$C$13</f>
+        <v>8.8576263988067352E-2</v>
+      </c>
+      <c r="F37" s="28">
+        <f>F30*$C$14</f>
+        <v>4.3997540899502405E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A38" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="28">
+        <f t="shared" ref="B38:B40" si="12">B31*$C$10</f>
+        <v>0.14242043914818325</v>
+      </c>
+      <c r="C38" s="28">
+        <f t="shared" ref="C38:C40" si="13">C31*$C$11</f>
+        <v>0.12574794106263337</v>
+      </c>
+      <c r="D38" s="28">
+        <f t="shared" ref="D38:D40" si="14">D31*$C$12</f>
+        <v>0.10511069241290988</v>
+      </c>
+      <c r="E38" s="28">
+        <f t="shared" ref="E38:E40" si="15">E31*$C$13</f>
+        <v>7.7022838250493345E-2</v>
+      </c>
+      <c r="F38" s="28">
+        <f t="shared" ref="F38:F40" si="16">F31*$C$14</f>
+        <v>4.986387968610273E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A39" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="28">
+        <f t="shared" si="12"/>
+        <v>0.1602229940417062</v>
+      </c>
+      <c r="C39" s="28">
+        <f t="shared" si="13"/>
+        <v>0.11501336072801832</v>
+      </c>
+      <c r="D39" s="28">
+        <f t="shared" si="14"/>
+        <v>9.3166295547806477E-2</v>
+      </c>
+      <c r="E39" s="28">
+        <f t="shared" si="15"/>
+        <v>6.9320554425444006E-2</v>
+      </c>
+      <c r="F39" s="28">
+        <f t="shared" si="16"/>
+        <v>5.1623781322082833E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A40" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="28">
+        <f t="shared" si="12"/>
+        <v>0.18311199319052135</v>
+      </c>
+      <c r="C40" s="28">
+        <f t="shared" si="13"/>
+        <v>0.10427878039340328</v>
+      </c>
+      <c r="D40" s="28">
+        <f t="shared" si="14"/>
+        <v>8.5999657428744436E-2</v>
+      </c>
+      <c r="E40" s="28">
+        <f t="shared" si="15"/>
+        <v>6.2581056078525849E-2</v>
+      </c>
+      <c r="F40" s="28">
+        <f t="shared" si="16"/>
+        <v>5.3970316836722945E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A44" s="5"/>
+      <c r="B44" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="28">
+        <v>0.10254271618669196</v>
+      </c>
+      <c r="C45" s="28">
+        <v>0.15028412468461064</v>
+      </c>
+      <c r="D45" s="28">
+        <v>0.11347177021848223</v>
+      </c>
+      <c r="E45" s="28">
+        <v>8.8576263988067352E-2</v>
+      </c>
+      <c r="F45" s="28">
+        <v>4.3997540899502405E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="28">
+        <v>0.14242043914818325</v>
+      </c>
+      <c r="C46" s="28">
+        <v>0.12574794106263337</v>
+      </c>
+      <c r="D46" s="28">
+        <v>0.10511069241290988</v>
+      </c>
+      <c r="E46" s="28">
+        <v>7.7022838250493345E-2</v>
+      </c>
+      <c r="F46" s="28">
+        <v>4.986387968610273E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A47" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47">
+        <f>IF(B45&gt;=B46,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:F47" si="17">IF(C45&gt;=C46,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A48" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" cm="1">
+        <f t="array" ref="B48:F48">TRANSPOSE($C$10:$C$14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="C48">
+        <v>0.25</v>
+      </c>
+      <c r="D48">
+        <v>0.2</v>
+      </c>
+      <c r="E48">
+        <v>0.15</v>
+      </c>
+      <c r="F48">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A49" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49">
+        <f>SUMPRODUCT(B47:F47,_xlfn.ANCHORARRAY(B48))</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A52" s="5"/>
+      <c r="B52" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E52" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A53" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="28">
+        <v>0.10254271618669196</v>
+      </c>
+      <c r="C53" s="28">
+        <v>0.15028412468461064</v>
+      </c>
+      <c r="D53" s="28">
+        <v>0.11347177021848223</v>
+      </c>
+      <c r="E53" s="28">
+        <v>8.8576263988067352E-2</v>
+      </c>
+      <c r="F53" s="28">
+        <v>4.3997540899502405E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A54" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="28">
+        <v>0.1602229940417062</v>
+      </c>
+      <c r="C54" s="28">
+        <v>0.11501336072801832</v>
+      </c>
+      <c r="D54" s="28">
+        <v>9.3166295547806477E-2</v>
+      </c>
+      <c r="E54" s="28">
+        <v>6.9320554425444006E-2</v>
+      </c>
+      <c r="F54" s="28">
+        <v>5.1623781322082833E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A55" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55">
+        <f>IF(B53&gt;=B54,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <f t="shared" ref="C55" si="18">IF(C53&gt;=C54,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ref="D55" si="19">IF(D53&gt;=D54,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55" si="20">IF(E53&gt;=E54,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ref="F55" si="21">IF(F53&gt;=F54,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A56" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" cm="1">
+        <f t="array" ref="B56:F56">TRANSPOSE($C$10:$C$14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="C56">
+        <v>0.25</v>
+      </c>
+      <c r="D56">
+        <v>0.2</v>
+      </c>
+      <c r="E56">
+        <v>0.15</v>
+      </c>
+      <c r="F56">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A57" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57">
+        <f>SUMPRODUCT(B55:F55,_xlfn.ANCHORARRAY(B56))</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A62" s="5"/>
+      <c r="B62" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A63" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="28">
+        <v>0.18311199319052135</v>
+      </c>
+      <c r="C63" s="28">
+        <v>0.10427878039340328</v>
+      </c>
+      <c r="D63" s="28">
+        <v>8.5999657428744436E-2</v>
+      </c>
+      <c r="E63" s="28">
+        <v>6.2581056078525849E-2</v>
+      </c>
+      <c r="F63" s="28">
+        <v>5.3970316836722945E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A64" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="28">
+        <v>0.1602229940417062</v>
+      </c>
+      <c r="C64" s="28">
+        <v>0.11501336072801832</v>
+      </c>
+      <c r="D64" s="28">
+        <v>9.3166295547806477E-2</v>
+      </c>
+      <c r="E64" s="28">
+        <v>6.9320554425444006E-2</v>
+      </c>
+      <c r="F64" s="28">
+        <v>5.1623781322082833E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A65" s="30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65">
+        <f>IF(B63&gt;=B64,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <f t="shared" ref="C65" si="22">IF(C63&gt;=C64,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ref="D65" si="23">IF(D63&gt;=D64,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <f t="shared" ref="E65" si="24">IF(E63&gt;=E64,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <f t="shared" ref="F65" si="25">IF(F63&gt;=F64,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A66" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" cm="1">
+        <f t="array" ref="B66:F66">TRANSPOSE($C$10:$C$14)</f>
+        <v>0.3</v>
+      </c>
+      <c r="C66">
+        <v>0.25</v>
+      </c>
+      <c r="D66">
+        <v>0.2</v>
+      </c>
+      <c r="E66">
+        <v>0.15</v>
+      </c>
+      <c r="F66">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A67" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C67">
+        <f>SUMPRODUCT(B65:F65,_xlfn.ANCHORARRAY(B66))</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A71" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B71" s="5">
+        <v>0</v>
+      </c>
+      <c r="C71" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D71" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A72" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C72" s="5">
+        <v>0</v>
+      </c>
+      <c r="D72" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A73" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="D73" s="5">
+        <v>0</v>
+      </c>
+      <c r="E73" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A74" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C74" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="D74" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E74" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A79" s="5"/>
+      <c r="B79" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C79" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F79" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A80" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B80" s="28">
+        <v>0.10254271618669196</v>
+      </c>
+      <c r="C80" s="28">
+        <v>0.15028412468461064</v>
+      </c>
+      <c r="D80" s="28">
+        <v>0.11347177021848223</v>
+      </c>
+      <c r="E80" s="28">
+        <v>8.8576263988067352E-2</v>
+      </c>
+      <c r="F80" s="28">
+        <v>4.3997540899502405E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A81" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="28">
+        <v>0.14242043914818325</v>
+      </c>
+      <c r="C81" s="28">
+        <v>0.12574794106263337</v>
+      </c>
+      <c r="D81" s="28">
+        <v>0.10511069241290988</v>
+      </c>
+      <c r="E81" s="28">
+        <v>7.7022838250493345E-2</v>
+      </c>
+      <c r="F81" s="28">
+        <v>4.986387968610273E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A82" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B82" s="29">
+        <f>MAX(B80:B81)-MIN(B80:B81)</f>
+        <v>3.9877722961491294E-2</v>
+      </c>
+      <c r="C82" s="29">
+        <f t="shared" ref="C82:F82" si="26">MAX(C80:C81)-MIN(C80:C81)</f>
+        <v>2.4536183621977264E-2</v>
+      </c>
+      <c r="D82" s="29">
+        <f t="shared" si="26"/>
+        <v>8.3610778055723534E-3</v>
+      </c>
+      <c r="E82" s="29">
+        <f t="shared" si="26"/>
+        <v>1.1553425737574008E-2</v>
+      </c>
+      <c r="F82" s="29">
+        <f t="shared" si="26"/>
+        <v>5.8663387866003253E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A83" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B83" s="29">
+        <f>MAX(B82:F82)</f>
+        <v>3.9877722961491294E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A86" s="5"/>
+      <c r="B86" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A87" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B87" s="28">
+        <v>0.18311199319052135</v>
+      </c>
+      <c r="C87" s="28">
+        <v>0.10427878039340328</v>
+      </c>
+      <c r="D87" s="28">
+        <v>8.5999657428744436E-2</v>
+      </c>
+      <c r="E87" s="28">
+        <v>6.2581056078525849E-2</v>
+      </c>
+      <c r="F87" s="28">
+        <v>5.3970316836722945E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A88" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="28">
+        <v>0.1602229940417062</v>
+      </c>
+      <c r="C88" s="28">
+        <v>0.11501336072801832</v>
+      </c>
+      <c r="D88" s="28">
+        <v>9.3166295547806477E-2</v>
+      </c>
+      <c r="E88" s="28">
+        <v>6.9320554425444006E-2</v>
+      </c>
+      <c r="F88" s="28">
+        <v>5.1623781322082833E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A89" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="B89" s="29">
+        <f>MAX(B87:B88)-MIN(B87:B88)</f>
+        <v>2.2888999148815148E-2</v>
+      </c>
+      <c r="C89" s="29">
+        <f t="shared" ref="C89" si="27">MAX(C87:C88)-MIN(C87:C88)</f>
+        <v>1.0734580334615038E-2</v>
+      </c>
+      <c r="D89" s="29">
+        <f t="shared" ref="D89" si="28">MAX(D87:D88)-MIN(D87:D88)</f>
+        <v>7.166638119062041E-3</v>
+      </c>
+      <c r="E89" s="29">
+        <f t="shared" ref="E89" si="29">MAX(E87:E88)-MIN(E87:E88)</f>
+        <v>6.7394983469181574E-3</v>
+      </c>
+      <c r="F89" s="29">
+        <f t="shared" ref="F89" si="30">MAX(F87:F88)-MIN(F87:F88)</f>
+        <v>2.3465355146401121E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A90" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B90" s="29">
+        <f>MAX(B89:F89)</f>
+        <v>2.2888999148815148E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>161</v>
+      </c>
+      <c r="B92">
+        <v>8.056927700382939E-2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A96" s="5"/>
+      <c r="B96" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C96" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D96" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E96" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F96" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A97" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B97" s="28">
+        <v>0.10254271618669196</v>
+      </c>
+      <c r="C97" s="28">
+        <v>0.15028412468461064</v>
+      </c>
+      <c r="D97" s="28">
+        <v>0.11347177021848223</v>
+      </c>
+      <c r="E97" s="28">
+        <v>8.8576263988067352E-2</v>
+      </c>
+      <c r="F97" s="28">
+        <v>4.3997540899502405E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A98" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B98" s="28">
+        <v>0.14242043914818325</v>
+      </c>
+      <c r="C98" s="28">
+        <v>0.12574794106263337</v>
+      </c>
+      <c r="D98" s="28">
+        <v>0.10511069241290988</v>
+      </c>
+      <c r="E98" s="28">
+        <v>7.7022838250493345E-2</v>
+      </c>
+      <c r="F98" s="28">
+        <v>4.986387968610273E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A99" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B99">
+        <f>IF(B97&lt;=B98,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <f t="shared" ref="C99:F99" si="31">IF(C97&lt;=C98,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A100" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B100" s="29">
+        <f>MAX(B97:B98)-MIN(B97:B98)</f>
+        <v>3.9877722961491294E-2</v>
+      </c>
+      <c r="C100" s="29">
+        <f t="shared" ref="C100:F100" si="32">MAX(C97:C98)-MIN(C97:C98)</f>
+        <v>2.4536183621977264E-2</v>
+      </c>
+      <c r="D100" s="29">
+        <f t="shared" si="32"/>
+        <v>8.3610778055723534E-3</v>
+      </c>
+      <c r="E100" s="29">
+        <f t="shared" si="32"/>
+        <v>1.1553425737574008E-2</v>
+      </c>
+      <c r="F100" s="29">
+        <f t="shared" si="32"/>
+        <v>5.8663387866003253E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A101" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C101" s="29">
+        <f>B100</f>
+        <v>3.9877722961491294E-2</v>
+      </c>
+      <c r="D101" s="29">
+        <f>F100</f>
+        <v>5.8663387866003253E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A102" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C102">
+        <f>MAX(C101:D101)/$B$92</f>
+        <v>0.49494949494949469</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A105" s="5"/>
+      <c r="B105" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C105" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D105" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E105" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F105" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A106" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B106" s="28">
+        <v>0.18311199319052135</v>
+      </c>
+      <c r="C106" s="28">
+        <v>0.10427878039340328</v>
+      </c>
+      <c r="D106" s="28">
+        <v>8.5999657428744436E-2</v>
+      </c>
+      <c r="E106" s="28">
+        <v>6.2581056078525849E-2</v>
+      </c>
+      <c r="F106" s="28">
+        <v>5.3970316836722945E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A107" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B107" s="28">
+        <v>0.1602229940417062</v>
+      </c>
+      <c r="C107" s="28">
+        <v>0.11501336072801832</v>
+      </c>
+      <c r="D107" s="28">
+        <v>9.3166295547806477E-2</v>
+      </c>
+      <c r="E107" s="28">
+        <v>6.9320554425444006E-2</v>
+      </c>
+      <c r="F107" s="28">
+        <v>5.1623781322082833E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A108" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B108">
+        <f>IF(B106&lt;=B107,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="C108">
+        <f t="shared" ref="C108" si="33">IF(C106&lt;=C107,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <f t="shared" ref="D108" si="34">IF(D106&lt;=D107,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <f t="shared" ref="E108" si="35">IF(E106&lt;=E107,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F108">
+        <f t="shared" ref="F108" si="36">IF(F106&lt;=F107,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A109" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B109" s="29">
+        <f>MAX(B106:B107)-MIN(B106:B107)</f>
+        <v>2.2888999148815148E-2</v>
+      </c>
+      <c r="C109" s="29">
+        <f t="shared" ref="C109:F109" si="37">MAX(C106:C107)-MIN(C106:C107)</f>
+        <v>1.0734580334615038E-2</v>
+      </c>
+      <c r="D109" s="29">
+        <f t="shared" si="37"/>
+        <v>7.166638119062041E-3</v>
+      </c>
+      <c r="E109" s="29">
+        <f t="shared" si="37"/>
+        <v>6.7394983469181574E-3</v>
+      </c>
+      <c r="F109" s="29">
+        <f t="shared" si="37"/>
+        <v>2.3465355146401121E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A110" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C110" s="29">
+        <f>C109</f>
+        <v>1.0734580334615038E-2</v>
+      </c>
+      <c r="D110" s="29">
+        <f>D109</f>
+        <v>7.166638119062041E-3</v>
+      </c>
+      <c r="E110" s="29">
+        <f>E109</f>
+        <v>6.7394983469181574E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A111" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="C111">
+        <f>MAX(C110:E110)/$B$92</f>
+        <v>0.13323416485547998</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A114" s="5"/>
+      <c r="B114" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A115" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B115" s="5">
+        <v>0</v>
+      </c>
+      <c r="C115" s="5">
+        <v>0.49494949494949397</v>
+      </c>
+      <c r="D115" s="5">
+        <v>0.71590909090909105</v>
+      </c>
+      <c r="E115" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A116" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B116" s="5">
+        <v>0.30453523395538301</v>
+      </c>
+      <c r="C116" s="5">
+        <v>0</v>
+      </c>
+      <c r="D116" s="5">
+        <v>0.22095959595959599</v>
+      </c>
+      <c r="E116" s="5">
+        <v>0.50505050505050497</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A117" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B117" s="5">
+        <v>0.43776939881086302</v>
+      </c>
+      <c r="C117" s="5">
+        <v>0.148250019229236</v>
+      </c>
+      <c r="D117" s="5">
+        <v>0</v>
+      </c>
+      <c r="E117" s="5">
+        <v>0.28409090909090801</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A118" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B118" s="5">
+        <v>0.57100356366634297</v>
+      </c>
+      <c r="C118" s="5">
+        <v>0.26646832971096002</v>
+      </c>
+      <c r="D118" s="5">
+        <v>0.13323416485547901</v>
+      </c>
+      <c r="E118" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>170</v>
+      </c>
+      <c r="C121">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>171</v>
+      </c>
+      <c r="C122">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>172</v>
+      </c>
+      <c r="D124" t="s">
+        <v>177</v>
+      </c>
+      <c r="E124" t="s">
+        <v>178</v>
+      </c>
+      <c r="F124" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>173</v>
+      </c>
+      <c r="C125" t="s">
+        <v>175</v>
+      </c>
+      <c r="D125">
+        <v>0.6</v>
+      </c>
+      <c r="E125">
+        <f>$C$121</f>
+        <v>0.5</v>
+      </c>
+      <c r="F125" t="b">
+        <f>D125&gt;=E125</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>174</v>
+      </c>
+      <c r="C126" t="s">
+        <v>176</v>
+      </c>
+      <c r="D126">
+        <v>0.49490000000000001</v>
+      </c>
+      <c r="E126">
+        <f>$C$122</f>
+        <v>0.5</v>
+      </c>
+      <c r="F126" t="b">
+        <f>D126&lt;=E126</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
+        <v>180</v>
+      </c>
+      <c r="C127" t="str">
+        <f>IF(AND(F125=TRUE,F126=TRUE),"Yes","No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
+        <v>181</v>
+      </c>
+      <c r="D129" t="s">
+        <v>177</v>
+      </c>
+      <c r="E129" t="s">
+        <v>178</v>
+      </c>
+      <c r="F129" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>173</v>
+      </c>
+      <c r="C130" t="s">
+        <v>175</v>
+      </c>
+      <c r="D130">
+        <v>0.6</v>
+      </c>
+      <c r="E130">
+        <f>$C$121</f>
+        <v>0.5</v>
+      </c>
+      <c r="F130" t="b">
+        <f>D130&gt;=E130</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" t="s">
+        <v>176</v>
+      </c>
+      <c r="D131">
+        <v>0.71589999999999998</v>
+      </c>
+      <c r="E131">
+        <f>$C$122</f>
+        <v>0.5</v>
+      </c>
+      <c r="F131" t="b">
+        <f>D131&lt;=E131</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A132" t="s">
+        <v>180</v>
+      </c>
+      <c r="C132" t="str">
+        <f>IF(AND(F130=TRUE,F131=TRUE),"Yes","No")</f>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E136" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A137" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" s="5">
+        <v>0</v>
+      </c>
+      <c r="C137" s="5">
+        <v>1</v>
+      </c>
+      <c r="D137" s="5">
+        <v>0</v>
+      </c>
+      <c r="E137" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A138" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="5">
+        <v>0</v>
+      </c>
+      <c r="C138" s="5">
+        <v>0</v>
+      </c>
+      <c r="D138" s="5">
+        <v>1</v>
+      </c>
+      <c r="E138" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A139" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139" s="5">
+        <v>0</v>
+      </c>
+      <c r="C139" s="5">
+        <v>0</v>
+      </c>
+      <c r="D139" s="5">
+        <v>0</v>
+      </c>
+      <c r="E139" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A140" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" s="5">
+        <v>0</v>
+      </c>
+      <c r="C140" s="5">
+        <v>0</v>
+      </c>
+      <c r="D140" s="5">
+        <v>0</v>
+      </c>
+      <c r="E140" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A142" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B143" t="s">
+        <v>184</v>
+      </c>
+      <c r="C143" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A144" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B144" s="31">
+        <v>1</v>
+      </c>
+      <c r="C144" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
+        <v>139</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
+        <v>140</v>
+      </c>
+      <c r="B146">
+        <v>1</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
+        <v>141</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add PROMETHEE decision-making notebook with supplier evaluation analysis
- Implemented decision matrix for supplier alternatives based on multiple criteria.
- Defined criteria weights and preference functions for evaluation.
- Calculated pairwise preference matrices for each criterion.
- Aggregated preferences to compute overall preference matrix.
- Performed PROMETHEE II flow calculations and generated final ranking.
- Included detailed output for each step to facilitate understanding of the decision-making process.
</commit_message>
<xml_diff>
--- a/data/01_examples_with_answer.xlsx
+++ b/data/01_examples_with_answer.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hecto\Desktop\code\mcdm\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35130070-FD82-4B7D-9F85-3259716CEB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CFBCEF-ED6E-4C0B-8BE2-84FBF38913E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="27634" windowHeight="16629" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SAW" sheetId="1" r:id="rId1"/>
     <sheet name="AHP" sheetId="2" r:id="rId2"/>
     <sheet name="ANP" sheetId="3" r:id="rId3"/>
     <sheet name="TOPSIS" sheetId="4" r:id="rId4"/>
-    <sheet name="ELECTRE" sheetId="5" r:id="rId5"/>
+    <sheet name="ELECTRE I" sheetId="5" r:id="rId5"/>
+    <sheet name="PROMETHEE II" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="1" hidden="1">AHP!$I$35:$I$39</definedName>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="225">
   <si>
     <t>Decision Matrix</t>
   </si>
@@ -649,6 +650,123 @@
   </si>
   <si>
     <t>Outranked by Count</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>A1_BasicCNC</t>
+  </si>
+  <si>
+    <t>A2_PrecisionCNC</t>
+  </si>
+  <si>
+    <t>A3_HighSpeedCNC</t>
+  </si>
+  <si>
+    <t>A4_IndustrialCNC</t>
+  </si>
+  <si>
+    <t>Step 1: Decision Matrix</t>
+  </si>
+  <si>
+    <t>Step 2: Criteria Weights</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Minimize</t>
+  </si>
+  <si>
+    <t>Precision Tolerance</t>
+  </si>
+  <si>
+    <t>Maximize</t>
+  </si>
+  <si>
+    <t>Step 3: Define Preference Thresholds (p) using Linear Preference</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Step 4: Compute Pairwise Preference</t>
+  </si>
+  <si>
+    <t>Criteria: Cost</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>A1 vs A2</t>
+  </si>
+  <si>
+    <t>A1 vs A3</t>
+  </si>
+  <si>
+    <t>A4 vs A3</t>
+  </si>
+  <si>
+    <t>Pairwise Preference Matrix: Cost</t>
+  </si>
+  <si>
+    <t>Pairwise Preference Matrix: Precision Tolerance</t>
+  </si>
+  <si>
+    <t>Power Consumption</t>
+  </si>
+  <si>
+    <t>Pairwise Preference Matrix: Speed</t>
+  </si>
+  <si>
+    <t>Pairwise Preference Matrix: Reliability</t>
+  </si>
+  <si>
+    <t>Pairwise Preference Matrix: Power Consumption</t>
+  </si>
+  <si>
+    <t>Step 5: Calculate Overall Preference Matrix π(a,b)</t>
+  </si>
+  <si>
+    <t>Higher values indicate stronger preference</t>
+  </si>
+  <si>
+    <t>Interpretation:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">π(A1,A2) = overall preference degree of A1 over A2 </t>
+  </si>
+  <si>
+    <t>Step 6: Calculate PROMETHEE Flows and Final Ranking</t>
+  </si>
+  <si>
+    <t>Positive Flow φ⁺</t>
+  </si>
+  <si>
+    <t>Negative Flow φ⁻</t>
+  </si>
+  <si>
+    <t>Positive Flow φ⁺ (dominance over others)</t>
+  </si>
+  <si>
+    <t>Net Flow φ (final score)</t>
+  </si>
+  <si>
+    <t>Negative Flow φ⁻ (dominated by others)</t>
+  </si>
+  <si>
+    <t>Net Flow φ</t>
+  </si>
+  <si>
+    <t>Sort the rankings</t>
   </si>
 </sst>
 </file>
@@ -774,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -810,6 +928,9 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -825,10 +946,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,20 +1287,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="K2" s="23" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="K2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -1224,7 +1341,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1245,7 +1362,7 @@
       <c r="G4" s="2">
         <v>7</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="5" t="s">
@@ -1273,7 +1390,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A5" s="24"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1409,7 @@
       <c r="G5" s="2">
         <v>9</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1318,7 +1435,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="24"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1337,7 +1454,7 @@
       <c r="G6" s="2">
         <v>8</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1363,7 +1480,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A7" s="24"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1382,7 +1499,7 @@
       <c r="G7" s="2">
         <v>10</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="27"/>
       <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1408,7 +1525,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A8" s="24"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1544,7 @@
       <c r="G8" s="2">
         <v>6</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1453,11 +1570,11 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1469,31 +1586,31 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="1">
         <v>0.25</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
     </row>
     <row r="12" spans="1:15" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="1">
         <v>0.3</v>
       </c>
@@ -1520,18 +1637,18 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
       <c r="D13" s="1">
         <v>0.2</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="27" t="s">
         <v>9</v>
       </c>
       <c r="J13" s="5" t="s">
@@ -1559,18 +1676,18 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
       <c r="D14" s="1">
         <v>0.15</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="5" t="s">
         <v>11</v>
       </c>
@@ -1596,18 +1713,18 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
       <c r="D15" s="1">
         <v>0.1</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="27"/>
       <c r="J15" s="5" t="s">
         <v>12</v>
       </c>
@@ -1634,7 +1751,7 @@
     </row>
     <row r="16" spans="1:15" ht="14.6" x14ac:dyDescent="0.4">
       <c r="D16" s="1"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="5" t="s">
         <v>13</v>
       </c>
@@ -1660,7 +1777,7 @@
       </c>
     </row>
     <row r="17" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I17" s="24"/>
+      <c r="I17" s="27"/>
       <c r="J17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1721,7 +1838,7 @@
       </c>
     </row>
     <row r="21" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I21" s="24" t="s">
+      <c r="I21" s="27" t="s">
         <v>9</v>
       </c>
       <c r="J21" s="5" t="s">
@@ -1737,7 +1854,7 @@
       </c>
     </row>
     <row r="22" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I22" s="24"/>
+      <c r="I22" s="27"/>
       <c r="J22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1868,7 @@
       </c>
     </row>
     <row r="23" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I23" s="24"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="5" t="s">
         <v>12</v>
       </c>
@@ -1765,7 +1882,7 @@
       </c>
     </row>
     <row r="24" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I24" s="24"/>
+      <c r="I24" s="27"/>
       <c r="J24" s="5" t="s">
         <v>13</v>
       </c>
@@ -1779,7 +1896,7 @@
       </c>
     </row>
     <row r="25" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I25" s="24"/>
+      <c r="I25" s="27"/>
       <c r="J25" s="5" t="s">
         <v>14</v>
       </c>
@@ -1810,7 +1927,7 @@
       </c>
     </row>
     <row r="28" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I28" s="24" t="s">
+      <c r="I28" s="27" t="s">
         <v>9</v>
       </c>
       <c r="J28" s="5" t="str">
@@ -1825,7 +1942,7 @@
       </c>
     </row>
     <row r="29" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I29" s="24"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="5" t="str">
         <v>Laptop B</v>
       </c>
@@ -1837,7 +1954,7 @@
       </c>
     </row>
     <row r="30" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I30" s="24"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="5" t="str">
         <v>Laptop D</v>
       </c>
@@ -1849,7 +1966,7 @@
       </c>
     </row>
     <row r="31" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I31" s="24"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="5" t="str">
         <v>Laptop E</v>
       </c>
@@ -1861,7 +1978,7 @@
       </c>
     </row>
     <row r="32" spans="9:15" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="I32" s="24"/>
+      <c r="I32" s="27"/>
       <c r="J32" s="5" t="str">
         <v>Laptop A</v>
       </c>
@@ -1919,19 +2036,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
       <c r="H1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
     </row>
     <row r="2" spans="1:14" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A2" s="5"/>
@@ -3062,36 +3179,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="F1" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="K1" s="27" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="K1" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="P1" s="27" t="s">
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="P1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="X1" s="27" t="s">
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="X1" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
     </row>
     <row r="2" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
@@ -3282,18 +3399,18 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="K6" s="27" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="K6" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
       <c r="P6" t="s">
         <v>9</v>
       </c>
@@ -3494,12 +3611,12 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
       <c r="P10" t="s">
         <v>66</v>
       </c>
@@ -3653,12 +3770,12 @@
       </c>
     </row>
     <row r="12" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
       <c r="F12" t="s">
         <v>72</v>
       </c>
@@ -4025,12 +4142,12 @@
       <c r="B16" s="13">
         <v>0.62501307434829401</v>
       </c>
-      <c r="P16" s="27" t="s">
+      <c r="P16" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="27"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
       <c r="X16" t="s">
         <v>68</v>
       </c>
@@ -4088,18 +4205,18 @@
         <f>SUM(B14:B16)</f>
         <v>1</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="K17" s="27" t="s">
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="K17" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
       <c r="P17" t="s">
         <v>84</v>
       </c>
@@ -4176,12 +4293,12 @@
       </c>
     </row>
     <row r="19" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="F19" t="s">
         <v>2</v>
       </c>
@@ -4284,7 +4401,7 @@
       <c r="B20" s="14">
         <v>3.01829470728963</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="30" t="s">
         <v>66</v>
       </c>
       <c r="G20" t="s">
@@ -4390,7 +4507,7 @@
         <f>(B20-COUNTA(A8:A10))/(COUNTA(A8:A10)-1)</f>
         <v>9.1473536448150039E-3</v>
       </c>
-      <c r="F21" s="27"/>
+      <c r="F21" s="30"/>
       <c r="G21" t="s">
         <v>68</v>
       </c>
@@ -4493,7 +4610,7 @@
       <c r="B22">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="30" t="s">
         <v>71</v>
       </c>
       <c r="G22" t="s">
@@ -4584,7 +4701,7 @@
         <f>B21/B22</f>
         <v>1.5771299387612077E-2</v>
       </c>
-      <c r="F23" s="27"/>
+      <c r="F23" s="30"/>
       <c r="G23" t="s">
         <v>68</v>
       </c>
@@ -4668,7 +4785,7 @@
       </c>
     </row>
     <row r="24" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="30" t="s">
         <v>72</v>
       </c>
       <c r="G24" t="s">
@@ -4754,7 +4871,7 @@
       </c>
     </row>
     <row r="25" spans="1:38" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="F25" s="27"/>
+      <c r="F25" s="30"/>
       <c r="G25" t="s">
         <v>68</v>
       </c>
@@ -5461,12 +5578,12 @@
     </row>
     <row r="43" spans="16:30" ht="14.6" x14ac:dyDescent="0.4"/>
     <row r="44" spans="16:30" ht="14.6" x14ac:dyDescent="0.4">
-      <c r="X44" s="27" t="s">
+      <c r="X44" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="Y44" s="27"/>
-      <c r="Z44" s="27"/>
-      <c r="AA44" s="27"/>
+      <c r="Y44" s="30"/>
+      <c r="Z44" s="30"/>
+      <c r="AA44" s="30"/>
     </row>
     <row r="45" spans="16:30" ht="14.6" x14ac:dyDescent="0.4">
       <c r="X45" t="s">
@@ -8259,8 +8376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC014023-8504-4C6E-827A-566A60E05094}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D142" sqref="D142"/>
+    <sheetView topLeftCell="A59" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -8480,7 +8597,7 @@
         <v>96.04000000000002</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ref="C18:F18" si="0">D3^2</f>
+        <f t="shared" ref="D18:F18" si="0">D3^2</f>
         <v>90.25</v>
       </c>
       <c r="E18" s="5">
@@ -8501,7 +8618,7 @@
         <v>3.0864197530864198E-7</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" ref="B19:F19" si="2">C4^2</f>
+        <f t="shared" ref="C19:F19" si="2">C4^2</f>
         <v>67.239999999999995</v>
       </c>
       <c r="D19" s="5">
@@ -8526,7 +8643,7 @@
         <v>3.9062500000000002E-7</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" ref="B20:F20" si="3">C5^2</f>
+        <f t="shared" ref="C20:F20" si="3">C5^2</f>
         <v>56.25</v>
       </c>
       <c r="D20" s="5">
@@ -8551,7 +8668,7 @@
         <v>5.1020408163265302E-7</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" ref="B21:F21" si="4">C6^2</f>
+        <f t="shared" ref="C21:F21" si="4">C6^2</f>
         <v>46.239999999999995</v>
       </c>
       <c r="D21" s="5">
@@ -8589,64 +8706,64 @@
         <f>SUM(B18:B21)</f>
         <v>1.369471056941295E-6</v>
       </c>
-      <c r="C24" s="28">
-        <f t="shared" ref="B24:F24" si="5">SUM(C18:C21)</f>
+      <c r="C24" s="23">
+        <f t="shared" ref="C24:F24" si="5">SUM(C18:C21)</f>
         <v>265.77000000000004</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="23">
         <f t="shared" si="5"/>
         <v>280.37</v>
       </c>
-      <c r="E24" s="28">
+      <c r="E24" s="23">
         <f t="shared" si="5"/>
         <v>242.73</v>
       </c>
-      <c r="F24" s="28">
+      <c r="F24" s="23">
         <f t="shared" si="5"/>
         <v>290.58</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="23" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B27" s="28">
+      <c r="B27" s="23">
         <f>SQRT(B24)</f>
         <v>1.1702440159818358E-3</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="23">
         <f t="shared" ref="C27:F27" si="6">SQRT(C24)</f>
         <v>16.302453803032229</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="23">
         <f t="shared" si="6"/>
         <v>16.744252745345193</v>
       </c>
-      <c r="E27" s="28">
+      <c r="E27" s="23">
         <f t="shared" si="6"/>
         <v>15.579794607118542</v>
       </c>
-      <c r="F27" s="28">
+      <c r="F27" s="23">
         <f t="shared" si="6"/>
         <v>17.046407246103207</v>
       </c>
@@ -8673,23 +8790,23 @@
       <c r="A30" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="23">
         <f>(1/B3)/$B$27</f>
         <v>0.34180905395563987</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="23">
         <f>C3/$C$27</f>
         <v>0.60113649873844255</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="23">
         <f>D3/$D$27</f>
         <v>0.56735885109241113</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="23">
         <f>E3/$E$27</f>
         <v>0.59050842658711566</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="23">
         <f>F3/$F$27</f>
         <v>0.43997540899502402</v>
       </c>
@@ -8698,23 +8815,23 @@
       <c r="A31" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="28">
+      <c r="B31" s="23">
         <f t="shared" ref="B31:B33" si="7">(1/B4)/$B$27</f>
         <v>0.4747347971606109</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="23">
         <f t="shared" ref="C31:C33" si="8">C4/$C$27</f>
         <v>0.50299176425053349</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="23">
         <f t="shared" ref="D31:D33" si="9">D4/$D$27</f>
         <v>0.52555346206454934</v>
       </c>
-      <c r="E31" s="28">
+      <c r="E31" s="23">
         <f t="shared" ref="E31:E33" si="10">E4/$E$27</f>
         <v>0.51348558833662228</v>
       </c>
-      <c r="F31" s="28">
+      <c r="F31" s="23">
         <f t="shared" ref="F31:F33" si="11">F4/$F$27</f>
         <v>0.49863879686102724</v>
       </c>
@@ -8723,23 +8840,23 @@
       <c r="A32" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="23">
         <f t="shared" si="7"/>
         <v>0.53407664680568734</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="23">
         <f t="shared" si="8"/>
         <v>0.46005344291207328</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="23">
         <f t="shared" si="9"/>
         <v>0.46583147773903233</v>
       </c>
-      <c r="E32" s="28">
+      <c r="E32" s="23">
         <f t="shared" si="10"/>
         <v>0.46213702950296009</v>
       </c>
-      <c r="F32" s="28">
+      <c r="F32" s="23">
         <f t="shared" si="11"/>
         <v>0.51623781322082829</v>
       </c>
@@ -8748,59 +8865,59 @@
       <c r="A33" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="28">
+      <c r="B33" s="23">
         <f t="shared" si="7"/>
         <v>0.61037331063507116</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="23">
         <f t="shared" si="8"/>
         <v>0.41711512157361313</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="23">
         <f t="shared" si="9"/>
         <v>0.42999828714372212</v>
       </c>
-      <c r="E33" s="28">
+      <c r="E33" s="23">
         <f t="shared" si="10"/>
         <v>0.41720704052350566</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="23">
         <f t="shared" si="11"/>
         <v>0.53970316836722942</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>144</v>
       </c>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="5"/>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F36" s="28" t="s">
+      <c r="F36" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -8808,23 +8925,23 @@
       <c r="A37" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="28">
+      <c r="B37" s="23">
         <f>B30*$C$10</f>
         <v>0.10254271618669196</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="23">
         <f>C30*$C$11</f>
         <v>0.15028412468461064</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="23">
         <f>D30*$C$12</f>
         <v>0.11347177021848223</v>
       </c>
-      <c r="E37" s="28">
+      <c r="E37" s="23">
         <f>E30*$C$13</f>
         <v>8.8576263988067352E-2</v>
       </c>
-      <c r="F37" s="28">
+      <c r="F37" s="23">
         <f>F30*$C$14</f>
         <v>4.3997540899502405E-2</v>
       </c>
@@ -8833,23 +8950,23 @@
       <c r="A38" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="23">
         <f t="shared" ref="B38:B40" si="12">B31*$C$10</f>
         <v>0.14242043914818325</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C38" s="23">
         <f t="shared" ref="C38:C40" si="13">C31*$C$11</f>
         <v>0.12574794106263337</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="23">
         <f t="shared" ref="D38:D40" si="14">D31*$C$12</f>
         <v>0.10511069241290988</v>
       </c>
-      <c r="E38" s="28">
+      <c r="E38" s="23">
         <f t="shared" ref="E38:E40" si="15">E31*$C$13</f>
         <v>7.7022838250493345E-2</v>
       </c>
-      <c r="F38" s="28">
+      <c r="F38" s="23">
         <f t="shared" ref="F38:F40" si="16">F31*$C$14</f>
         <v>4.986387968610273E-2</v>
       </c>
@@ -8858,23 +8975,23 @@
       <c r="A39" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B39" s="28">
+      <c r="B39" s="23">
         <f t="shared" si="12"/>
         <v>0.1602229940417062</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="23">
         <f t="shared" si="13"/>
         <v>0.11501336072801832</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="23">
         <f t="shared" si="14"/>
         <v>9.3166295547806477E-2</v>
       </c>
-      <c r="E39" s="28">
+      <c r="E39" s="23">
         <f t="shared" si="15"/>
         <v>6.9320554425444006E-2</v>
       </c>
-      <c r="F39" s="28">
+      <c r="F39" s="23">
         <f t="shared" si="16"/>
         <v>5.1623781322082833E-2</v>
       </c>
@@ -8883,23 +9000,23 @@
       <c r="A40" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="28">
+      <c r="B40" s="23">
         <f t="shared" si="12"/>
         <v>0.18311199319052135</v>
       </c>
-      <c r="C40" s="28">
+      <c r="C40" s="23">
         <f t="shared" si="13"/>
         <v>0.10427878039340328</v>
       </c>
-      <c r="D40" s="28">
+      <c r="D40" s="23">
         <f t="shared" si="14"/>
         <v>8.5999657428744436E-2</v>
       </c>
-      <c r="E40" s="28">
+      <c r="E40" s="23">
         <f t="shared" si="15"/>
         <v>6.2581056078525849E-2</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="23">
         <f t="shared" si="16"/>
         <v>5.3970316836722945E-2</v>
       </c>
@@ -8916,19 +9033,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D44" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -8936,19 +9053,19 @@
       <c r="A45" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="28">
+      <c r="B45" s="23">
         <v>0.10254271618669196</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C45" s="23">
         <v>0.15028412468461064</v>
       </c>
-      <c r="D45" s="28">
+      <c r="D45" s="23">
         <v>0.11347177021848223</v>
       </c>
-      <c r="E45" s="28">
+      <c r="E45" s="23">
         <v>8.8576263988067352E-2</v>
       </c>
-      <c r="F45" s="28">
+      <c r="F45" s="23">
         <v>4.3997540899502405E-2</v>
       </c>
     </row>
@@ -8956,24 +9073,24 @@
       <c r="A46" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="23">
         <v>0.14242043914818325</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C46" s="23">
         <v>0.12574794106263337</v>
       </c>
-      <c r="D46" s="28">
+      <c r="D46" s="23">
         <v>0.10511069241290988</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="23">
         <v>7.7022838250493345E-2</v>
       </c>
-      <c r="F46" s="28">
+      <c r="F46" s="23">
         <v>4.986387968610273E-2</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A47" s="30" t="s">
+      <c r="A47" t="s">
         <v>147</v>
       </c>
       <c r="B47">
@@ -8998,7 +9115,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A48" s="30" t="s">
+      <c r="A48" t="s">
         <v>15</v>
       </c>
       <c r="B48" cm="1">
@@ -9019,7 +9136,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A49" s="30" t="s">
+      <c r="A49" t="s">
         <v>148</v>
       </c>
       <c r="C49">
@@ -9034,19 +9151,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" s="5"/>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D52" s="28" t="s">
+      <c r="D52" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F52" s="28" t="s">
+      <c r="F52" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9054,19 +9171,19 @@
       <c r="A53" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="28">
+      <c r="B53" s="23">
         <v>0.10254271618669196</v>
       </c>
-      <c r="C53" s="28">
+      <c r="C53" s="23">
         <v>0.15028412468461064</v>
       </c>
-      <c r="D53" s="28">
+      <c r="D53" s="23">
         <v>0.11347177021848223</v>
       </c>
-      <c r="E53" s="28">
+      <c r="E53" s="23">
         <v>8.8576263988067352E-2</v>
       </c>
-      <c r="F53" s="28">
+      <c r="F53" s="23">
         <v>4.3997540899502405E-2</v>
       </c>
     </row>
@@ -9074,24 +9191,24 @@
       <c r="A54" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="23">
         <v>0.1602229940417062</v>
       </c>
-      <c r="C54" s="28">
+      <c r="C54" s="23">
         <v>0.11501336072801832</v>
       </c>
-      <c r="D54" s="28">
+      <c r="D54" s="23">
         <v>9.3166295547806477E-2</v>
       </c>
-      <c r="E54" s="28">
+      <c r="E54" s="23">
         <v>6.9320554425444006E-2</v>
       </c>
-      <c r="F54" s="28">
+      <c r="F54" s="23">
         <v>5.1623781322082833E-2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A55" s="30" t="s">
+      <c r="A55" t="s">
         <v>150</v>
       </c>
       <c r="B55">
@@ -9116,7 +9233,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A56" s="30" t="s">
+      <c r="A56" t="s">
         <v>15</v>
       </c>
       <c r="B56" cm="1">
@@ -9137,7 +9254,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A57" s="30" t="s">
+      <c r="A57" t="s">
         <v>151</v>
       </c>
       <c r="C57">
@@ -9157,19 +9274,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" s="5"/>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="28" t="s">
+      <c r="D62" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E62" s="28" t="s">
+      <c r="E62" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F62" s="28" t="s">
+      <c r="F62" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9177,19 +9294,19 @@
       <c r="A63" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B63" s="28">
+      <c r="B63" s="23">
         <v>0.18311199319052135</v>
       </c>
-      <c r="C63" s="28">
+      <c r="C63" s="23">
         <v>0.10427878039340328</v>
       </c>
-      <c r="D63" s="28">
+      <c r="D63" s="23">
         <v>8.5999657428744436E-2</v>
       </c>
-      <c r="E63" s="28">
+      <c r="E63" s="23">
         <v>6.2581056078525849E-2</v>
       </c>
-      <c r="F63" s="28">
+      <c r="F63" s="23">
         <v>5.3970316836722945E-2</v>
       </c>
     </row>
@@ -9197,24 +9314,24 @@
       <c r="A64" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B64" s="28">
+      <c r="B64" s="23">
         <v>0.1602229940417062</v>
       </c>
-      <c r="C64" s="28">
+      <c r="C64" s="23">
         <v>0.11501336072801832</v>
       </c>
-      <c r="D64" s="28">
+      <c r="D64" s="23">
         <v>9.3166295547806477E-2</v>
       </c>
-      <c r="E64" s="28">
+      <c r="E64" s="23">
         <v>6.9320554425444006E-2</v>
       </c>
-      <c r="F64" s="28">
+      <c r="F64" s="23">
         <v>5.1623781322082833E-2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A65" s="30" t="s">
+      <c r="A65" t="s">
         <v>147</v>
       </c>
       <c r="B65">
@@ -9239,7 +9356,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A66" s="30" t="s">
+      <c r="A66" t="s">
         <v>15</v>
       </c>
       <c r="B66" cm="1">
@@ -9260,7 +9377,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A67" s="30" t="s">
+      <c r="A67" t="s">
         <v>152</v>
       </c>
       <c r="C67">
@@ -9373,19 +9490,19 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79" s="5"/>
-      <c r="B79" s="28" t="s">
+      <c r="B79" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C79" s="28" t="s">
+      <c r="C79" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D79" s="28" t="s">
+      <c r="D79" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E79" s="28" t="s">
+      <c r="E79" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F79" s="28" t="s">
+      <c r="F79" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9393,19 +9510,19 @@
       <c r="A80" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="28">
+      <c r="B80" s="23">
         <v>0.10254271618669196</v>
       </c>
-      <c r="C80" s="28">
+      <c r="C80" s="23">
         <v>0.15028412468461064</v>
       </c>
-      <c r="D80" s="28">
+      <c r="D80" s="23">
         <v>0.11347177021848223</v>
       </c>
-      <c r="E80" s="28">
+      <c r="E80" s="23">
         <v>8.8576263988067352E-2</v>
       </c>
-      <c r="F80" s="28">
+      <c r="F80" s="23">
         <v>4.3997540899502405E-2</v>
       </c>
     </row>
@@ -9413,52 +9530,52 @@
       <c r="A81" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B81" s="28">
+      <c r="B81" s="23">
         <v>0.14242043914818325</v>
       </c>
-      <c r="C81" s="28">
+      <c r="C81" s="23">
         <v>0.12574794106263337</v>
       </c>
-      <c r="D81" s="28">
+      <c r="D81" s="23">
         <v>0.10511069241290988</v>
       </c>
-      <c r="E81" s="28">
+      <c r="E81" s="23">
         <v>7.7022838250493345E-2</v>
       </c>
-      <c r="F81" s="28">
+      <c r="F81" s="23">
         <v>4.986387968610273E-2</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A82" s="30" t="s">
+      <c r="A82" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="29">
+      <c r="B82" s="24">
         <f>MAX(B80:B81)-MIN(B80:B81)</f>
         <v>3.9877722961491294E-2</v>
       </c>
-      <c r="C82" s="29">
+      <c r="C82" s="24">
         <f t="shared" ref="C82:F82" si="26">MAX(C80:C81)-MIN(C80:C81)</f>
         <v>2.4536183621977264E-2</v>
       </c>
-      <c r="D82" s="29">
+      <c r="D82" s="24">
         <f t="shared" si="26"/>
         <v>8.3610778055723534E-3</v>
       </c>
-      <c r="E82" s="29">
+      <c r="E82" s="24">
         <f t="shared" si="26"/>
         <v>1.1553425737574008E-2</v>
       </c>
-      <c r="F82" s="29">
+      <c r="F82" s="24">
         <f t="shared" si="26"/>
         <v>5.8663387866003253E-3</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A83" s="30" t="s">
+      <c r="A83" t="s">
         <v>158</v>
       </c>
-      <c r="B83" s="29">
+      <c r="B83" s="24">
         <f>MAX(B82:F82)</f>
         <v>3.9877722961491294E-2</v>
       </c>
@@ -9475,19 +9592,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86" s="5"/>
-      <c r="B86" s="28" t="s">
+      <c r="B86" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C86" s="28" t="s">
+      <c r="C86" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D86" s="28" t="s">
+      <c r="D86" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E86" s="28" t="s">
+      <c r="E86" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9495,19 +9612,19 @@
       <c r="A87" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B87" s="28">
+      <c r="B87" s="23">
         <v>0.18311199319052135</v>
       </c>
-      <c r="C87" s="28">
+      <c r="C87" s="23">
         <v>0.10427878039340328</v>
       </c>
-      <c r="D87" s="28">
+      <c r="D87" s="23">
         <v>8.5999657428744436E-2</v>
       </c>
-      <c r="E87" s="28">
+      <c r="E87" s="23">
         <v>6.2581056078525849E-2</v>
       </c>
-      <c r="F87" s="28">
+      <c r="F87" s="23">
         <v>5.3970316836722945E-2</v>
       </c>
     </row>
@@ -9515,52 +9632,52 @@
       <c r="A88" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B88" s="28">
+      <c r="B88" s="23">
         <v>0.1602229940417062</v>
       </c>
-      <c r="C88" s="28">
+      <c r="C88" s="23">
         <v>0.11501336072801832</v>
       </c>
-      <c r="D88" s="28">
+      <c r="D88" s="23">
         <v>9.3166295547806477E-2</v>
       </c>
-      <c r="E88" s="28">
+      <c r="E88" s="23">
         <v>6.9320554425444006E-2</v>
       </c>
-      <c r="F88" s="28">
+      <c r="F88" s="23">
         <v>5.1623781322082833E-2</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A89" s="30" t="s">
+      <c r="A89" t="s">
         <v>157</v>
       </c>
-      <c r="B89" s="29">
+      <c r="B89" s="24">
         <f>MAX(B87:B88)-MIN(B87:B88)</f>
         <v>2.2888999148815148E-2</v>
       </c>
-      <c r="C89" s="29">
+      <c r="C89" s="24">
         <f t="shared" ref="C89" si="27">MAX(C87:C88)-MIN(C87:C88)</f>
         <v>1.0734580334615038E-2</v>
       </c>
-      <c r="D89" s="29">
+      <c r="D89" s="24">
         <f t="shared" ref="D89" si="28">MAX(D87:D88)-MIN(D87:D88)</f>
         <v>7.166638119062041E-3</v>
       </c>
-      <c r="E89" s="29">
+      <c r="E89" s="24">
         <f t="shared" ref="E89" si="29">MAX(E87:E88)-MIN(E87:E88)</f>
         <v>6.7394983469181574E-3</v>
       </c>
-      <c r="F89" s="29">
+      <c r="F89" s="24">
         <f t="shared" ref="F89" si="30">MAX(F87:F88)-MIN(F87:F88)</f>
         <v>2.3465355146401121E-3</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A90" s="30" t="s">
+      <c r="A90" t="s">
         <v>158</v>
       </c>
-      <c r="B90" s="29">
+      <c r="B90" s="24">
         <f>MAX(B89:F89)</f>
         <v>2.2888999148815148E-2</v>
       </c>
@@ -9588,19 +9705,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A96" s="5"/>
-      <c r="B96" s="28" t="s">
+      <c r="B96" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C96" s="28" t="s">
+      <c r="C96" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D96" s="28" t="s">
+      <c r="D96" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E96" s="28" t="s">
+      <c r="E96" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F96" s="28" t="s">
+      <c r="F96" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9608,19 +9725,19 @@
       <c r="A97" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B97" s="28">
+      <c r="B97" s="23">
         <v>0.10254271618669196</v>
       </c>
-      <c r="C97" s="28">
+      <c r="C97" s="23">
         <v>0.15028412468461064</v>
       </c>
-      <c r="D97" s="28">
+      <c r="D97" s="23">
         <v>0.11347177021848223</v>
       </c>
-      <c r="E97" s="28">
+      <c r="E97" s="23">
         <v>8.8576263988067352E-2</v>
       </c>
-      <c r="F97" s="28">
+      <c r="F97" s="23">
         <v>4.3997540899502405E-2</v>
       </c>
     </row>
@@ -9628,24 +9745,24 @@
       <c r="A98" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B98" s="28">
+      <c r="B98" s="23">
         <v>0.14242043914818325</v>
       </c>
-      <c r="C98" s="28">
+      <c r="C98" s="23">
         <v>0.12574794106263337</v>
       </c>
-      <c r="D98" s="28">
+      <c r="D98" s="23">
         <v>0.10511069241290988</v>
       </c>
-      <c r="E98" s="28">
+      <c r="E98" s="23">
         <v>7.7022838250493345E-2</v>
       </c>
-      <c r="F98" s="28">
+      <c r="F98" s="23">
         <v>4.986387968610273E-2</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A99" s="30" t="s">
+      <c r="A99" t="s">
         <v>164</v>
       </c>
       <c r="B99">
@@ -9670,45 +9787,45 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A100" s="30" t="s">
+      <c r="A100" t="s">
         <v>165</v>
       </c>
-      <c r="B100" s="29">
+      <c r="B100" s="24">
         <f>MAX(B97:B98)-MIN(B97:B98)</f>
         <v>3.9877722961491294E-2</v>
       </c>
-      <c r="C100" s="29">
+      <c r="C100" s="24">
         <f t="shared" ref="C100:F100" si="32">MAX(C97:C98)-MIN(C97:C98)</f>
         <v>2.4536183621977264E-2</v>
       </c>
-      <c r="D100" s="29">
+      <c r="D100" s="24">
         <f t="shared" si="32"/>
         <v>8.3610778055723534E-3</v>
       </c>
-      <c r="E100" s="29">
+      <c r="E100" s="24">
         <f t="shared" si="32"/>
         <v>1.1553425737574008E-2</v>
       </c>
-      <c r="F100" s="29">
+      <c r="F100" s="24">
         <f t="shared" si="32"/>
         <v>5.8663387866003253E-3</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A101" s="30" t="s">
+      <c r="A101" t="s">
         <v>166</v>
       </c>
-      <c r="C101" s="29">
+      <c r="C101" s="24">
         <f>B100</f>
         <v>3.9877722961491294E-2</v>
       </c>
-      <c r="D101" s="29">
+      <c r="D101" s="24">
         <f>F100</f>
         <v>5.8663387866003253E-3</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A102" s="30" t="s">
+      <c r="A102" t="s">
         <v>167</v>
       </c>
       <c r="C102">
@@ -9728,19 +9845,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A105" s="5"/>
-      <c r="B105" s="28" t="s">
+      <c r="B105" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C105" s="28" t="s">
+      <c r="C105" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="D105" s="28" t="s">
+      <c r="D105" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E105" s="28" t="s">
+      <c r="E105" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F105" s="28" t="s">
+      <c r="F105" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -9748,19 +9865,19 @@
       <c r="A106" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B106" s="28">
+      <c r="B106" s="23">
         <v>0.18311199319052135</v>
       </c>
-      <c r="C106" s="28">
+      <c r="C106" s="23">
         <v>0.10427878039340328</v>
       </c>
-      <c r="D106" s="28">
+      <c r="D106" s="23">
         <v>8.5999657428744436E-2</v>
       </c>
-      <c r="E106" s="28">
+      <c r="E106" s="23">
         <v>6.2581056078525849E-2</v>
       </c>
-      <c r="F106" s="28">
+      <c r="F106" s="23">
         <v>5.3970316836722945E-2</v>
       </c>
     </row>
@@ -9768,24 +9885,24 @@
       <c r="A107" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B107" s="28">
+      <c r="B107" s="23">
         <v>0.1602229940417062</v>
       </c>
-      <c r="C107" s="28">
+      <c r="C107" s="23">
         <v>0.11501336072801832</v>
       </c>
-      <c r="D107" s="28">
+      <c r="D107" s="23">
         <v>9.3166295547806477E-2</v>
       </c>
-      <c r="E107" s="28">
+      <c r="E107" s="23">
         <v>6.9320554425444006E-2</v>
       </c>
-      <c r="F107" s="28">
+      <c r="F107" s="23">
         <v>5.1623781322082833E-2</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A108" s="30" t="s">
+      <c r="A108" t="s">
         <v>164</v>
       </c>
       <c r="B108">
@@ -9810,49 +9927,49 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A109" s="30" t="s">
+      <c r="A109" t="s">
         <v>165</v>
       </c>
-      <c r="B109" s="29">
+      <c r="B109" s="24">
         <f>MAX(B106:B107)-MIN(B106:B107)</f>
         <v>2.2888999148815148E-2</v>
       </c>
-      <c r="C109" s="29">
+      <c r="C109" s="24">
         <f t="shared" ref="C109:F109" si="37">MAX(C106:C107)-MIN(C106:C107)</f>
         <v>1.0734580334615038E-2</v>
       </c>
-      <c r="D109" s="29">
+      <c r="D109" s="24">
         <f t="shared" si="37"/>
         <v>7.166638119062041E-3</v>
       </c>
-      <c r="E109" s="29">
+      <c r="E109" s="24">
         <f t="shared" si="37"/>
         <v>6.7394983469181574E-3</v>
       </c>
-      <c r="F109" s="29">
+      <c r="F109" s="24">
         <f t="shared" si="37"/>
         <v>2.3465355146401121E-3</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A110" s="30" t="s">
+      <c r="A110" t="s">
         <v>166</v>
       </c>
-      <c r="C110" s="29">
+      <c r="C110" s="24">
         <f>C109</f>
         <v>1.0734580334615038E-2</v>
       </c>
-      <c r="D110" s="29">
+      <c r="D110" s="24">
         <f>D109</f>
         <v>7.166638119062041E-3</v>
       </c>
-      <c r="E110" s="29">
+      <c r="E110" s="24">
         <f>E109</f>
         <v>6.7394983469181574E-3</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A111" s="30" t="s">
+      <c r="A111" t="s">
         <v>167</v>
       </c>
       <c r="C111">
@@ -10198,13 +10315,13 @@
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A144" s="31" t="s">
+      <c r="A144" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="B144" s="31">
+      <c r="B144" s="25">
         <v>1</v>
       </c>
-      <c r="C144" s="31">
+      <c r="C144" s="25">
         <v>0</v>
       </c>
     </row>
@@ -10244,6 +10361,1187 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08EDF42-47F8-4493-8404-E9FD3A364E31}">
+  <dimension ref="A1:I87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.3828125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.61328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.15234375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.61328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.3828125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="5">
+        <v>120</v>
+      </c>
+      <c r="C3" s="5">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2000</v>
+      </c>
+      <c r="F3" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="5">
+        <v>180</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A5" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="5">
+        <v>150</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>40</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2800</v>
+      </c>
+      <c r="F5" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A6" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="5">
+        <v>200</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5">
+        <v>35</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4200</v>
+      </c>
+      <c r="F6" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>193</v>
+      </c>
+      <c r="F8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>194</v>
+      </c>
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>0.25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11">
+        <v>0.3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>186</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>197</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13">
+        <v>0.2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14">
+        <v>0.05</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" t="s">
+        <v>205</v>
+      </c>
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A20" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="5">
+        <v>120</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="5">
+        <v>120</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" s="5">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="5">
+        <v>180</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" s="5">
+        <v>150</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I21" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H22" t="s">
+        <v>194</v>
+      </c>
+      <c r="I22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B23">
+        <f>IF(B22="Maximize",B20-B21,B21-B20)</f>
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23">
+        <f>IF(E22="Maximize",E20-E21,E21-E20)</f>
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23">
+        <f>IF(I22="Maximize",I20-I21,I21-I20)</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>199</v>
+      </c>
+      <c r="I24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25">
+        <f>IF(B23&lt;=0,0,IF(B23&gt;=B24,1,B23/B24))</f>
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>202</v>
+      </c>
+      <c r="E25">
+        <f>IF(E23&lt;=0,0,IF(E23&gt;=E24,1,E23/E24))</f>
+        <v>0.6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>202</v>
+      </c>
+      <c r="I25">
+        <f>IF(I23&lt;=0,0,IF(I23&gt;=I24,1,I23/I24))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A30" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A31" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A32" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A37" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A38" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A39" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A50" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0</v>
+      </c>
+      <c r="C50" s="5">
+        <v>0</v>
+      </c>
+      <c r="D50" s="5">
+        <v>0</v>
+      </c>
+      <c r="E50" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A51" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A52" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="5">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="C52" s="5">
+        <v>0</v>
+      </c>
+      <c r="D52" s="5">
+        <v>0</v>
+      </c>
+      <c r="E52" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A53" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="5">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="D53" s="5">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="E53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A57" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0</v>
+      </c>
+      <c r="C57" s="5">
+        <v>0</v>
+      </c>
+      <c r="D57" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="E57" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A58" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.375</v>
+      </c>
+      <c r="C58" s="5">
+        <v>0</v>
+      </c>
+      <c r="D58" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A59" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0</v>
+      </c>
+      <c r="C59" s="5">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5">
+        <v>0</v>
+      </c>
+      <c r="E59" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A60" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="C60" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D60" s="5">
+        <v>1</v>
+      </c>
+      <c r="E60" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A64" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64" s="23">
+        <f>B29*$B$10+B36*$B$11+B43*$B$12+B50*$B$13+B57*$B$14</f>
+        <v>0</v>
+      </c>
+      <c r="C64" s="23">
+        <f t="shared" ref="C64:E64" si="0">C29*$B$10+C36*$B$11+C43*$B$12+C50*$B$13+C57*$B$14</f>
+        <v>0.3</v>
+      </c>
+      <c r="D64" s="23">
+        <f t="shared" si="0"/>
+        <v>0.16875000000000001</v>
+      </c>
+      <c r="E64" s="23">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A65" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" s="23">
+        <f t="shared" ref="B65:E66" si="1">B30*$B$10+B37*$B$11+B44*$B$12+B51*$B$13+B58*$B$14</f>
+        <v>0.51875000000000004</v>
+      </c>
+      <c r="C65" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D65" s="23">
+        <f t="shared" si="1"/>
+        <v>0.31089999999999995</v>
+      </c>
+      <c r="E65" s="23">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A66" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" s="23">
+        <f t="shared" ref="B66:E66" si="2">B31*$B$10+B38*$B$11+B45*$B$12+B52*$B$13+B59*$B$14</f>
+        <v>0.37660000000000005</v>
+      </c>
+      <c r="C66" s="23">
+        <f>C31*$B$10+C38*$B$11+C45*$B$12+C52*$B$13+C59*$B$14</f>
+        <v>0.35</v>
+      </c>
+      <c r="D66" s="23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E66" s="23">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A67" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67" s="23">
+        <f t="shared" ref="B67:E67" si="3">B32*$B$10+B39*$B$11+B46*$B$12+B53*$B$13+B60*$B$14</f>
+        <v>0.63125000000000009</v>
+      </c>
+      <c r="C67" s="23">
+        <f t="shared" si="3"/>
+        <v>0.37590000000000007</v>
+      </c>
+      <c r="D67" s="23">
+        <f t="shared" si="3"/>
+        <v>0.53660000000000008</v>
+      </c>
+      <c r="E67" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" t="s">
+        <v>219</v>
+      </c>
+      <c r="D73" t="s">
+        <v>223</v>
+      </c>
+      <c r="E73" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A74" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B74" s="23">
+        <f>SUM(B64:E64)/3</f>
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="C74" s="23">
+        <f>SUM(B64:B67)/3</f>
+        <v>0.50886666666666669</v>
+      </c>
+      <c r="D74" s="23">
+        <f>B74-C74</f>
+        <v>-0.26928333333333332</v>
+      </c>
+      <c r="E74" s="5">
+        <f>_xlfn.RANK.EQ(D74,$D$74:$D$77)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A75" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B75" s="23">
+        <f t="shared" ref="B75:B77" si="4">SUM(B65:E65)/3</f>
+        <v>0.30988333333333334</v>
+      </c>
+      <c r="C75" s="23">
+        <f>SUM(C64:C67)/3</f>
+        <v>0.3419666666666667</v>
+      </c>
+      <c r="D75" s="23">
+        <f t="shared" ref="D75:D77" si="5">B75-C75</f>
+        <v>-3.2083333333333353E-2</v>
+      </c>
+      <c r="E75" s="5">
+        <f t="shared" ref="E75:E77" si="6">_xlfn.RANK.EQ(D75,$D$74:$D$77)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A76" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B76" s="23">
+        <f t="shared" si="4"/>
+        <v>0.3422</v>
+      </c>
+      <c r="C76" s="23">
+        <f>SUM(D64:D67)/3</f>
+        <v>0.33875000000000005</v>
+      </c>
+      <c r="D76" s="23">
+        <f t="shared" si="5"/>
+        <v>3.4499999999999531E-3</v>
+      </c>
+      <c r="E76" s="5">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A77" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="23">
+        <f t="shared" si="4"/>
+        <v>0.51458333333333339</v>
+      </c>
+      <c r="C77" s="23">
+        <f>SUM(E64:E67)/3</f>
+        <v>0.21666666666666665</v>
+      </c>
+      <c r="D77" s="23">
+        <f t="shared" si="5"/>
+        <v>0.29791666666666672</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>103</v>
+      </c>
+      <c r="B83" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" t="s">
+        <v>219</v>
+      </c>
+      <c r="D83" t="s">
+        <v>223</v>
+      </c>
+      <c r="E83" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A84" s="5" t="str" cm="1">
+        <f t="array" ref="A84:E87">_xlfn._xlws.SORT($A$74:$E$77,5)</f>
+        <v>A4_IndustrialCNC</v>
+      </c>
+      <c r="B84" s="23">
+        <v>0.51458333333333339</v>
+      </c>
+      <c r="C84" s="23">
+        <v>0.21666666666666665</v>
+      </c>
+      <c r="D84" s="23">
+        <v>0.29791666666666672</v>
+      </c>
+      <c r="E84" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A85" s="5" t="str">
+        <v>A3_HighSpeedCNC</v>
+      </c>
+      <c r="B85" s="23">
+        <v>0.3422</v>
+      </c>
+      <c r="C85" s="23">
+        <v>0.33875000000000005</v>
+      </c>
+      <c r="D85" s="23">
+        <v>3.4499999999999531E-3</v>
+      </c>
+      <c r="E85" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A86" s="5" t="str">
+        <v>A2_PrecisionCNC</v>
+      </c>
+      <c r="B86" s="23">
+        <v>0.30988333333333334</v>
+      </c>
+      <c r="C86" s="23">
+        <v>0.3419666666666667</v>
+      </c>
+      <c r="D86" s="23">
+        <v>-3.2083333333333353E-2</v>
+      </c>
+      <c r="E86" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A87" s="5" t="str">
+        <v>A1_BasicCNC</v>
+      </c>
+      <c r="B87" s="23">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="C87" s="23">
+        <v>0.50886666666666669</v>
+      </c>
+      <c r="D87" s="23">
+        <v>-0.26928333333333332</v>
+      </c>
+      <c r="E87" s="5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>